<commit_message>
Remove extra fields from delivery and clean up logic in registration form
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/deliveries/forms/deliveries/deliveries.xlsx
+++ b/appGreece/config/tables/deliveries/forms/deliveries/deliveries.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/appGreece/config/tables/deliveries/forms/deliveries/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="989" activeTab="3"/>
+    <workbookView xWindow="3160" yWindow="620" windowWidth="44000" windowHeight="23200" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="5" r:id="rId1"/>
@@ -20,13 +15,13 @@
     <sheet name="calculates" sheetId="6" r:id="rId6"/>
     <sheet name="properties" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -36,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="112">
   <si>
     <t>type</t>
   </si>
@@ -294,12 +289,6 @@
   </si>
   <si>
     <t>now()</t>
-  </si>
-  <si>
-    <t>What is the name of the distributor?</t>
-  </si>
-  <si>
-    <t>What is the name of the delivery site?</t>
   </si>
   <si>
     <t>thanks</t>
@@ -987,7 +976,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -995,13 +984,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="53.83203125" customWidth="1"/>
@@ -1015,7 +1004,7 @@
     <col min="10" max="10" width="48.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="23">
       <c r="A1" s="6" t="s">
         <v>47</v>
       </c>
@@ -1050,9 +1039,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="23">
       <c r="A2" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="37"/>
@@ -1062,7 +1051,7 @@
       <c r="G2" s="39"/>
       <c r="H2" s="40"/>
     </row>
-    <row r="3" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="23">
       <c r="A3" s="9"/>
       <c r="B3" s="17"/>
       <c r="C3" s="18" t="s">
@@ -1091,7 +1080,7 @@
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
     </row>
-    <row r="4" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="23">
       <c r="A4" s="22"/>
       <c r="B4" s="23"/>
       <c r="C4" s="24" t="s">
@@ -1123,9 +1112,9 @@
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
     </row>
-    <row r="5" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="23">
       <c r="A5" s="22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
@@ -1148,7 +1137,7 @@
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
     </row>
-    <row r="6" spans="1:21" ht="48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="46">
       <c r="A6" s="22" t="s">
         <v>62</v>
       </c>
@@ -1177,7 +1166,7 @@
       <c r="T6" s="11"/>
       <c r="U6" s="11"/>
     </row>
-    <row r="7" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="23">
       <c r="A7" s="22"/>
       <c r="B7" s="23"/>
       <c r="C7" s="24" t="s">
@@ -1188,7 +1177,7 @@
         <v>66</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="26"/>
@@ -1209,7 +1198,7 @@
       <c r="T7" s="11"/>
       <c r="U7" s="11"/>
     </row>
-    <row r="8" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="23">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -1241,7 +1230,7 @@
       <c r="T8" s="11"/>
       <c r="U8" s="11"/>
     </row>
-    <row r="9" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="23">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
@@ -1272,7 +1261,7 @@
       <c r="T9" s="11"/>
       <c r="U9" s="11"/>
     </row>
-    <row r="10" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="23">
       <c r="A10" s="22" t="s">
         <v>69</v>
       </c>
@@ -1297,7 +1286,7 @@
       <c r="T10" s="11"/>
       <c r="U10" s="11"/>
     </row>
-    <row r="11" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="23">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
@@ -1324,7 +1313,7 @@
       <c r="T11" s="11"/>
       <c r="U11" s="11"/>
     </row>
-    <row r="12" spans="1:21" ht="43" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="41">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
@@ -1356,7 +1345,7 @@
       <c r="T12" s="11"/>
       <c r="U12" s="11"/>
     </row>
-    <row r="13" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="23">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24" t="s">
@@ -1388,7 +1377,7 @@
       <c r="T13" s="11"/>
       <c r="U13" s="11"/>
     </row>
-    <row r="14" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="23">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
@@ -1417,7 +1406,7 @@
       <c r="T14" s="11"/>
       <c r="U14" s="11"/>
     </row>
-    <row r="15" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="23">
       <c r="A15" s="22" t="s">
         <v>73</v>
       </c>
@@ -1442,7 +1431,7 @@
       <c r="T15" s="11"/>
       <c r="U15" s="11"/>
     </row>
-    <row r="16" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="23">
       <c r="A16" s="22" t="s">
         <v>62</v>
       </c>
@@ -1469,7 +1458,7 @@
       <c r="T16" s="11"/>
       <c r="U16" s="11"/>
     </row>
-    <row r="17" spans="1:21" ht="43" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="41">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
@@ -1503,7 +1492,7 @@
       <c r="T17" s="11"/>
       <c r="U17" s="11"/>
     </row>
-    <row r="18" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="23">
       <c r="A18" s="22" t="s">
         <v>62</v>
       </c>
@@ -1530,7 +1519,7 @@
       <c r="T18" s="11"/>
       <c r="U18" s="11"/>
     </row>
-    <row r="19" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="23">
       <c r="A19" s="22" t="s">
         <v>79</v>
       </c>
@@ -1555,7 +1544,7 @@
       <c r="T19" s="11"/>
       <c r="U19" s="11"/>
     </row>
-    <row r="20" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="23">
       <c r="A20" s="22" t="s">
         <v>73</v>
       </c>
@@ -1580,7 +1569,7 @@
       <c r="T20" s="11"/>
       <c r="U20" s="11"/>
     </row>
-    <row r="21" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="23">
       <c r="A21" s="22" t="s">
         <v>69</v>
       </c>
@@ -1605,7 +1594,7 @@
       <c r="T21" s="11"/>
       <c r="U21" s="11"/>
     </row>
-    <row r="22" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="23">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="24" t="s">
@@ -1632,7 +1621,7 @@
       <c r="T22" s="11"/>
       <c r="U22" s="11"/>
     </row>
-    <row r="23" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="23">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="24" t="s">
@@ -1663,7 +1652,7 @@
       <c r="T23" s="11"/>
       <c r="U23" s="11"/>
     </row>
-    <row r="24" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="23">
       <c r="A24" s="22" t="s">
         <v>73</v>
       </c>
@@ -1688,12 +1677,12 @@
       <c r="T24" s="11"/>
       <c r="U24" s="11"/>
     </row>
-    <row r="25" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="23">
       <c r="A25" s="22" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
@@ -1715,7 +1704,7 @@
       <c r="T25" s="11"/>
       <c r="U25" s="11"/>
     </row>
-    <row r="26" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="23">
       <c r="A26" s="22"/>
       <c r="B26" s="23"/>
       <c r="C26" s="24" t="s">
@@ -1744,7 +1733,7 @@
       <c r="T26" s="11"/>
       <c r="U26" s="11"/>
     </row>
-    <row r="27" spans="1:21" ht="43" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="41">
       <c r="A27" s="22"/>
       <c r="B27" s="23"/>
       <c r="C27" s="24" t="s">
@@ -1773,7 +1762,7 @@
       <c r="T27" s="11"/>
       <c r="U27" s="11"/>
     </row>
-    <row r="28" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="23">
       <c r="A28" s="22"/>
       <c r="B28" s="23"/>
       <c r="C28" s="24" t="s">
@@ -1802,18 +1791,18 @@
       <c r="T28" s="11"/>
       <c r="U28" s="11"/>
     </row>
-    <row r="29" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="41">
       <c r="A29" s="22"/>
       <c r="B29" s="23"/>
       <c r="C29" s="24" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="D29" s="24"/>
       <c r="E29" s="4" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G29" s="25"/>
       <c r="H29" s="26"/>
@@ -1831,19 +1820,15 @@
       <c r="T29" s="11"/>
       <c r="U29" s="11"/>
     </row>
-    <row r="30" spans="1:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
+    <row r="30" spans="1:21" ht="23">
+      <c r="A30" s="22" t="s">
+        <v>69</v>
+      </c>
       <c r="B30" s="23"/>
-      <c r="C30" s="24" t="s">
-        <v>3</v>
-      </c>
+      <c r="C30" s="24"/>
       <c r="D30" s="24"/>
-      <c r="E30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>87</v>
-      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="32"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
       <c r="I30" s="11"/>
@@ -1860,18 +1845,20 @@
       <c r="T30" s="11"/>
       <c r="U30" s="11"/>
     </row>
-    <row r="31" spans="1:21" ht="43" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" ht="23">
       <c r="A31" s="22"/>
       <c r="B31" s="23"/>
       <c r="C31" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="24"/>
+        <v>75</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="E31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="32" t="s">
         <v>88</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>89</v>
       </c>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
@@ -1889,11 +1876,13 @@
       <c r="T31" s="11"/>
       <c r="U31" s="11"/>
     </row>
-    <row r="32" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="23">
       <c r="A32" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="23"/>
+        <v>62</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>78</v>
+      </c>
       <c r="C32" s="24"/>
       <c r="D32" s="24"/>
       <c r="E32" s="4"/>
@@ -1914,21 +1903,15 @@
       <c r="T32" s="11"/>
       <c r="U32" s="11"/>
     </row>
-    <row r="33" spans="1:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
+    <row r="33" spans="1:21" ht="23">
+      <c r="A33" s="22" t="s">
+        <v>79</v>
+      </c>
       <c r="B33" s="23"/>
-      <c r="C33" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F33" s="32" t="s">
-        <v>90</v>
-      </c>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
       <c r="I33" s="11"/>
@@ -1945,13 +1928,11 @@
       <c r="T33" s="11"/>
       <c r="U33" s="11"/>
     </row>
-    <row r="34" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" ht="23">
       <c r="A34" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>78</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B34" s="23"/>
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="4"/>
@@ -1972,15 +1953,19 @@
       <c r="T34" s="11"/>
       <c r="U34" s="11"/>
     </row>
-    <row r="35" spans="1:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="A35" s="22" t="s">
-        <v>79</v>
-      </c>
+    <row r="35" spans="1:21" ht="41">
+      <c r="A35" s="22"/>
       <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
+      <c r="C35" s="24" t="s">
+        <v>56</v>
+      </c>
       <c r="D35" s="24"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="32"/>
+      <c r="E35" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>90</v>
+      </c>
       <c r="G35" s="25"/>
       <c r="H35" s="26"/>
       <c r="I35" s="11"/>
@@ -1997,15 +1982,15 @@
       <c r="T35" s="11"/>
       <c r="U35" s="11"/>
     </row>
-    <row r="36" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" ht="23">
       <c r="A36" s="22" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B36" s="23"/>
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="32"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="33"/>
       <c r="G36" s="25"/>
       <c r="H36" s="26"/>
       <c r="I36" s="11"/>
@@ -2022,19 +2007,15 @@
       <c r="T36" s="11"/>
       <c r="U36" s="11"/>
     </row>
-    <row r="37" spans="1:21" ht="43" x14ac:dyDescent="0.3">
-      <c r="A37" s="22"/>
+    <row r="37" spans="1:21" ht="23">
+      <c r="A37" s="22" t="s">
+        <v>73</v>
+      </c>
       <c r="B37" s="23"/>
-      <c r="C37" s="24" t="s">
-        <v>56</v>
-      </c>
+      <c r="C37" s="24"/>
       <c r="D37" s="24"/>
-      <c r="E37" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F37" s="32" t="s">
-        <v>92</v>
-      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="32"/>
       <c r="G37" s="25"/>
       <c r="H37" s="26"/>
       <c r="I37" s="11"/>
@@ -2051,59 +2032,14 @@
       <c r="T37" s="11"/>
       <c r="U37" s="11"/>
     </row>
-    <row r="38" spans="1:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="A38" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
-      <c r="S38" s="11"/>
-      <c r="T38" s="11"/>
-      <c r="U38" s="11"/>
-    </row>
-    <row r="39" spans="1:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="A39" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="11"/>
-      <c r="T39" s="11"/>
-      <c r="U39" s="11"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2112,17 +2048,17 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2133,7 +2069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="23">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2141,7 +2077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="23">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2149,7 +2085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="23">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2157,7 +2093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="23">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2165,7 +2101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="23">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -2173,7 +2109,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="23">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -2181,7 +2117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="23">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -2189,7 +2125,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="23">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -2197,7 +2133,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="23">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
@@ -2205,7 +2141,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="23">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -2213,7 +2149,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="23">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -2221,7 +2157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="23">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -2229,7 +2165,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="23">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -2237,7 +2173,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="23">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
@@ -2245,7 +2181,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="23">
       <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
@@ -2253,7 +2189,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="23">
       <c r="A17" s="12" t="s">
         <v>3</v>
       </c>
@@ -2264,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="23">
       <c r="A18" s="12" t="s">
         <v>3</v>
       </c>
@@ -2275,7 +2211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="23">
       <c r="A19" s="12" t="s">
         <v>3</v>
       </c>
@@ -2286,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="23">
       <c r="A20" s="44" t="s">
         <v>3</v>
       </c>
@@ -2300,6 +2236,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2311,14 +2252,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="3" max="3" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="23">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -2329,7 +2270,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="23">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -2338,7 +2279,7 @@
       </c>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="23">
       <c r="A3" s="8" t="s">
         <v>27</v>
       </c>
@@ -2347,7 +2288,7 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="23">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -2356,7 +2297,7 @@
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="23">
       <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
@@ -2365,7 +2306,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="23">
       <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
@@ -2377,6 +2318,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2384,18 +2330,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2403,7 +2349,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -2411,7 +2357,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2419,7 +2365,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2427,7 +2373,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2435,7 +2381,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2446,6 +2392,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2457,14 +2408,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -2475,7 +2426,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -2486,7 +2437,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -2500,6 +2451,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2511,39 +2467,44 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="128.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="288" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="270">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="288" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="270">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2555,7 +2516,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
@@ -2564,15 +2525,15 @@
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>0</v>
@@ -2581,32 +2542,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>103</v>
-      </c>
-      <c r="B3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" t="s">
-        <v>105</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -2615,25 +2576,30 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
         <v>104</v>
-      </c>
-      <c r="C4" t="s">
-        <v>106</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>